<commit_message>
Initial commit for ner-sports-certificate project
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1068,7 +1068,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Basketball</t>
+          <t>Basketball competition,2011</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Rowing</t>
+          <t>Rowing competition,2011</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Karate</t>
+          <t>Karate competition,2011</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2432,7 +2432,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Boxing</t>
+          <t>Boxing competition,2011</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Weightlifting</t>
+          <t>Weightlifting competition,2012</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Boxing</t>
+          <t>Boxing competition,2011</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Basketball</t>
+          <t>Basketball competition,2011</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Badminton</t>
+          <t>Badminton competition,2011</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Triathlon</t>
+          <t>Triathlon competition,2012</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Weightlifting</t>
+          <t>Weightlifting competition,2011</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Weightlifting</t>
+          <t>Weightlifting competition,2011</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -5802,7 +5802,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Handball</t>
+          <t>Handball competition,2011</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Judo</t>
+          <t>Judo competition,2011</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -7308,7 +7308,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Badminton</t>
+          <t>Badminton competition,2011</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
@@ -7420,7 +7420,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Hockey</t>
+          <t>Hockey competition,2011</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -7472,7 +7472,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Softball</t>
+          <t>Softball competition,2011</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -7670,7 +7670,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Athletics</t>
+          <t>Athletics competition,2011</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -8512,7 +8512,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Triathlon</t>
+          <t>Triathlon competition,2012</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -8838,7 +8838,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Volleyball</t>
+          <t>Volleyball competition,2011</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -9242,7 +9242,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Taekwondo</t>
+          <t>Taekwondo competition,2011</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -9500,7 +9500,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Taekwondo</t>
+          <t>Taekwondo competition,2012</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -10068,7 +10068,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Volleyball</t>
+          <t>Volleyball competition,2011</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
@@ -10244,7 +10244,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Weightlifting</t>
+          <t>Weightlifting competition,2012</t>
         </is>
       </c>
       <c r="E344" t="inlineStr">
@@ -10352,7 +10352,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Taekwondo</t>
+          <t>Taekwondo competition,2011</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
@@ -10434,7 +10434,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Rowing</t>
+          <t>Rowing competition,2011</t>
         </is>
       </c>
       <c r="E351" t="inlineStr">
@@ -10894,7 +10894,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Badminton</t>
+          <t>Badminton competition,2011</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
@@ -11264,7 +11264,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Tennis</t>
+          <t>Tennis competition,2011</t>
         </is>
       </c>
       <c r="E380" t="inlineStr">
@@ -12060,7 +12060,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>Triathlon</t>
+          <t>Triathlon competition,2011</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -12766,7 +12766,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>Softball</t>
+          <t>Softball competition,2011</t>
         </is>
       </c>
       <c r="E433" t="inlineStr">
@@ -13184,7 +13184,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>Rowing</t>
+          <t>Rowing competition,2011</t>
         </is>
       </c>
       <c r="E448" t="inlineStr">
@@ -13210,7 +13210,7 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>Judo</t>
+          <t>Judo competition,2011</t>
         </is>
       </c>
       <c r="E449" t="inlineStr">

</xml_diff>